<commit_message>
Update Academic Services and Awards
</commit_message>
<xml_diff>
--- a/data/achievement.xlsx
+++ b/data/achievement.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56582C0B-91AB-4A38-AD8D-B1D03F51595C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B9E0DC-B884-4BD7-83BC-00539A791B1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="200">
   <si>
     <t>date</t>
   </si>
@@ -709,6 +709,30 @@
   </si>
   <si>
     <t>ACM CHI 2020 Papers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-09-17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaetano Borriello Outstanding Award Finalist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UbiComp/ISWC 2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designing Interactive Technologies to Encourage Physical Activities for Health Behavior Promotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACM HEALTH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1120,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1185,6 +1209,20 @@
         <v>193</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="18">
+        <v>43983</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1301,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2506EC-EE0F-4FFE-A52A-81C20650DD9B}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1338,79 +1376,97 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="13">
-        <v>2016</v>
+        <v>194</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>164</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="13" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B3" s="13">
         <v>2016</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="14"/>
+        <v>163</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="13" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B4" s="13">
         <v>2016</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="13">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D5" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B6" s="14">
         <v>2015</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F6" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>